<commit_message>
added PDF form R scraping section
</commit_message>
<xml_diff>
--- a/tables/Power_app_criteria.xlsx
+++ b/tables/Power_app_criteria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAlstad\Documents\Github_C\e-deviceIEP\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E3B260-E72A-4284-8EC8-1652B3F0FBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66102FB-8AEA-4CB4-9173-054363AD9C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29640" yWindow="1755" windowWidth="27960" windowHeight="11385" activeTab="5" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
+    <workbookView xWindow="3165" yWindow="705" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="5" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
   </bookViews>
   <sheets>
     <sheet name="Forms_Options" sheetId="1" r:id="rId1"/>
@@ -643,10 +643,6 @@
     <t>Per User Premium License (non-Gov't)</t>
   </si>
   <si>
-    <t>The 'Power Apps per User Premium Plan for Government' is an app developer license which is ~ $17/month; 
-The 'Power Apps per App Plan for Government' is the end-user license which is initiated when an app is shared with a new user; this license is ~$10/month for each user</t>
-  </si>
-  <si>
     <t>$10/Active User/month</t>
   </si>
   <si>
@@ -663,6 +659,10 @@
   </si>
   <si>
     <t xml:space="preserve">Drawing-on/ Annotating photo </t>
+  </si>
+  <si>
+    <t>The Power Apps per USER Premium Plan for Government' is an app developer license which is approx $17/mo.
+The Power Apps per APP Plan for Government is the end-user license which is initiated when an app is shared with a new user. This license is approx $10/mo for each user</t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1700,7 @@
         <v>69</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>113</v>
@@ -1739,13 +1739,13 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="18"/>
@@ -1880,7 +1880,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>110</v>
@@ -1990,7 +1990,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,7 +2029,7 @@
         <v>117</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="1" t="s">
@@ -2046,7 +2046,7 @@
         <v>128</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>91</v>
@@ -2063,7 +2063,7 @@
         <v>129</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>89</v>
@@ -2098,6 +2098,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>